<commit_message>
Adjust ALPS motifs of Nup157 / Nup170
</commit_message>
<xml_diff>
--- a/data_nic96/rmfs/XL_Nic96complex_structured.xlsx
+++ b/data_nic96/rmfs/XL_Nic96complex_structured.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20680" yWindow="0" windowWidth="18400" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="XL_Nic96complex_structured.csv" sheetId="1" r:id="rId1"/>
@@ -101,12 +101,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,8 +129,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -471,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -591,7 +598,7 @@
       <c r="C5">
         <v>266</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>517</v>
       </c>
       <c r="E5">
@@ -617,7 +624,7 @@
       <c r="C6">
         <v>275</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>378</v>
       </c>
       <c r="E6">
@@ -744,7 +751,7 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>378</v>
       </c>
       <c r="D11">
@@ -770,10 +777,10 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>378</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>446</v>
       </c>
       <c r="E12">
@@ -796,10 +803,10 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>389</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>361</v>
       </c>
       <c r="E13">
@@ -822,7 +829,7 @@
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>446</v>
       </c>
       <c r="D14">
@@ -848,10 +855,10 @@
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>446</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>526</v>
       </c>
       <c r="E15">
@@ -874,7 +881,7 @@
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>517</v>
       </c>
       <c r="D16">
@@ -900,10 +907,10 @@
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>517</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>529</v>
       </c>
       <c r="E17">
@@ -929,7 +936,7 @@
       <c r="C18">
         <v>543</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>527</v>
       </c>
       <c r="E18">

</xml_diff>